<commit_message>
Super cambio de diseño mas menu popup
</commit_message>
<xml_diff>
--- a/Proyecto/AplicacionPrincipal/bin/Debug/InformeBeneficiarios.xlsx
+++ b/Proyecto/AplicacionPrincipal/bin/Debug/InformeBeneficiarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Informe de Beneficiarios</t>
   </si>
@@ -81,6 +81,24 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Riquelme</t>
+  </si>
+  <si>
+    <t>Juan Roman</t>
+  </si>
+  <si>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>1010000001</t>
+  </si>
+  <si>
+    <t>boca@juniors.net</t>
+  </si>
+  <si>
+    <t>Secundario</t>
   </si>
 </sst>
 </file>
@@ -139,8 +157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSalesman" displayName="tblSalesman" ref="B4:I6" headerRowCount="1">
-  <autoFilter ref="B4:I6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblSalesman" displayName="tblSalesman" ref="B4:I7" headerRowCount="1">
+  <autoFilter ref="B4:I7"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Apellido"/>
@@ -157,7 +175,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:I6"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -166,7 +184,7 @@
     <col min="1" max="1" width="9.140625" customWidth="1" style="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1" style="1"/>
     <col min="3" max="3" width="11.3786566598075" customWidth="1" style="1"/>
-    <col min="4" max="4" width="11.3367107936314" customWidth="1" style="1"/>
+    <col min="4" max="4" width="13.6209368024554" customWidth="1" style="1"/>
     <col min="5" max="5" width="11.0131432669503" customWidth="1" style="1"/>
     <col min="6" max="6" width="14.6133095877511" customWidth="1" style="1"/>
     <col min="7" max="7" width="18.6073564801897" customWidth="1" style="1"/>
@@ -279,6 +297,32 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:I2"/>

</xml_diff>